<commit_message>
added K_means clustering for customer segmentation and streamlit dashboard for rfm values in tables , pie chart and scatterplot
</commit_message>
<xml_diff>
--- a/category_summary.xlsx
+++ b/category_summary.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,24 +422,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Cluster</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
-          <t>Customer Count</t>
+          <t>Recency_Mean</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t>Frequency_Mean</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
-          <t>Monetary</t>
+          <t>Monetary_Mean</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Customer_Count</t>
         </is>
       </c>
     </row>
@@ -460,13 +453,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>279</v>
+        <v>71.14</v>
       </c>
       <c r="C2" t="n">
         <v>8.5</v>
       </c>
       <c r="D2" t="n">
         <v>3226.84</v>
+      </c>
+      <c r="E2" t="n">
+        <v>279</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +470,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>103</v>
+        <v>547.89</v>
       </c>
       <c r="C3" t="n">
         <v>3.71</v>
       </c>
       <c r="D3" t="n">
         <v>1432.86</v>
+      </c>
+      <c r="E3" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +487,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>68</v>
+        <v>120.71</v>
       </c>
       <c r="C4" t="n">
         <v>8.210000000000001</v>
       </c>
       <c r="D4" t="n">
         <v>9236.450000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +504,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>343</v>
+        <v>98.81999999999999</v>
       </c>
       <c r="C5" t="n">
         <v>4.7</v>
       </c>
       <c r="D5" t="n">
         <v>1707.24</v>
+      </c>
+      <c r="E5" t="n">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>